<commit_message>
spp goal updated with ESA terrestrial plants and animals
</commit_message>
<xml_diff>
--- a/prep/CW/cw_impared_waters.xlsx
+++ b/prep/CW/cw_impared_waters.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents and Settings\eschemmel\Documents\github\mhi\prep\CW\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="510" windowWidth="23955" windowHeight="10035"/>
+    <workbookView minimized="1" xWindow="10230" yWindow="510" windowWidth="23955" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -27,12 +32,6 @@
     <t>n_impaired</t>
   </si>
   <si>
-    <t>percent_impared_water_state</t>
-  </si>
-  <si>
-    <t>percent_impared_island</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -49,12 +48,18 @@
   </si>
   <si>
     <t>2008-2010</t>
+  </si>
+  <si>
+    <t>percent_impared_water_island</t>
+  </si>
+  <si>
+    <t>percent_impared_state</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,##0\ \ \ \ \ \ \ "/>
     <numFmt numFmtId="165" formatCode="#,##0\ \ \ \ \ \ \ \ "/>
@@ -126,6 +131,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -173,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,9 +214,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -241,6 +266,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -420,13 +462,15 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -434,7 +478,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -443,10 +487,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -551,7 +595,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>2012</v>
@@ -571,7 +615,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>2012</v>
@@ -591,7 +635,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>2012</v>
@@ -611,10 +655,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="5">
         <v>176</v>
@@ -631,10 +675,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
         <v>81</v>
@@ -651,10 +695,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1">
         <v>176</v>
@@ -671,10 +715,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
         <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
       </c>
       <c r="C13" s="1">
         <v>89</v>
@@ -691,7 +735,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>2006</v>
@@ -711,7 +755,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>2006</v>
@@ -731,7 +775,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>2006</v>
@@ -751,7 +795,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>2006</v>

</xml_diff>